<commit_message>
Performance testing using NBench
</commit_message>
<xml_diff>
--- a/OutReachServiceLayer/ExcelReports/EventSummary_1st Dec PM-Christmas fair to save a school swimming pool.xlsx
+++ b/OutReachServiceLayer/ExcelReports/EventSummary_1st Dec PM-Christmas fair to save a school swimming pool.xlsx
@@ -67,10 +67,10 @@
     <x:t>United Kingdom</x:t>
   </x:si>
   <x:si>
-    <x:t>Okay</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Unexpected Personal Commitment</x:t>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>Unexpected Official Work</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -491,14 +491,30 @@
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="2"/>
-      <x:c r="B3" s="2"/>
-      <x:c r="C3" s="2"/>
-      <x:c r="D3" s="2"/>
-      <x:c r="E3" s="2"/>
-      <x:c r="F3" s="2"/>
-      <x:c r="G3" s="2"/>
-      <x:c r="H3" s="2"/>
+      <x:c r="A3" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="n">
+        <x:v>243742</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
     </x:row>
     <x:row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A4" s="2"/>

</xml_diff>